<commit_message>
Forçar alteração de senha dos usuários e edição dos dados do usuário logado
</commit_message>
<xml_diff>
--- a/storage/files/modelo_person.xlsx
+++ b/storage/files/modelo_person.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">sector</t>
   </si>
   <si>
-    <t xml:space="preserve">bithday</t>
+    <t xml:space="preserve">birthday</t>
   </si>
   <si>
     <t xml:space="preserve">gender</t>
@@ -174,7 +174,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -182,7 +182,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.2"/>
@@ -195,7 +195,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.53"/>
   </cols>

</xml_diff>